<commit_message>
commit STRING data files for individual proteins
</commit_message>
<xml_diff>
--- a/Data/string/A0A087WVF3_string.xlsx
+++ b/Data/string/A0A087WVF3_string.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cf5805afcc9bf9ef/Documents/!USF/^NBioinformatics/Applied Bioinformatics/Project/String data files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\USF Bioinformatics\GMS7930 Applied Bioinformatics\Research Human Core Duplicon Gene Families\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90EB62E2-361D-4154-9508-E57D2BEAE4A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76792E1-1066-49C2-8F7E-3590ACF5BCE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{5A5C50AE-401E-4449-ABA0-51DC3B46C602}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{86C82BCB-24EA-4973-8E7D-BA56AF1E05B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,13 +59,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF404040"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -88,8 +94,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,72 +415,72 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{093A2E15-C99B-429F-962B-603167E513ED}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{103910F3-898D-4EC3-B5DB-7343A7FBD5D3}">
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4">
+    <row r="3" spans="1:1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
+    <row r="5" spans="1:1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>3.12</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
+    <row r="7" spans="1:1" ht="51" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>0.93700000000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
+    <row r="9" spans="1:1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
+    <row r="11" spans="1:1" ht="51" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>9.0600000000000003E-3</v>
       </c>
     </row>
@@ -478,72 +490,72 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1D389AA-2D36-422C-8FB8-19251B9F9561}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9532D5C-EEFB-40D3-8891-0C23BDC286D8}">
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
+    <row r="3" spans="1:1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="51" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="51" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>0.5</v>
       </c>
     </row>
@@ -553,72 +565,72 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7AD954B-5B91-404D-B03D-678179C4E71E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164BA62A-843C-433D-8E34-8780CC4DA5A2}">
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
+    <row r="3" spans="1:1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="51" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="51" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>